<commit_message>
included TACS for stellar visibility calculation
TACS from Michael Cretignier
</commit_message>
<xml_diff>
--- a/results/Overlap_with_HWO_M_earth_2025.08.22.xlsx
+++ b/results/Overlap_with_HWO_M_earth_2025.08.22.xlsx
@@ -750,10 +750,10 @@
         <v>185.8487974986299</v>
       </c>
       <c r="R2" t="n">
-        <v>0.06072655052096795</v>
+        <v>0.03962970724823796</v>
       </c>
       <c r="S2" t="n">
-        <v>0.4325579507481528</v>
+        <v>0.2822841872127762</v>
       </c>
       <c r="T2" t="n">
         <v>0.03314148419589402</v>
@@ -771,7 +771,7 @@
         <v>0.2545505546694897</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.3198016311788879</v>
+        <v>0.2087002293461784</v>
       </c>
       <c r="Z2" t="n">
         <v>2.675178851982804</v>
@@ -896,10 +896,10 @@
         <v>245.7629703836871</v>
       </c>
       <c r="R3" t="n">
-        <v>0.06402164542916261</v>
+        <v>0.03403676776602877</v>
       </c>
       <c r="S3" t="n">
-        <v>0.5087125620470453</v>
+        <v>0.2704543317808828</v>
       </c>
       <c r="T3" t="n">
         <v>0.02531460317846459</v>
@@ -917,7 +917,7 @@
         <v>0.309247207436402</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.3371105966081873</v>
+        <v>0.1792230582532586</v>
       </c>
       <c r="Z3" t="n">
         <v>1.833398606190053</v>
@@ -1037,10 +1037,10 @@
         <v>233.8618542705035</v>
       </c>
       <c r="R4" t="n">
-        <v>0.05749566268718269</v>
+        <v>0.02729781493871667</v>
       </c>
       <c r="S4" t="n">
-        <v>0.4646115037941509</v>
+        <v>0.2205884453924024</v>
       </c>
       <c r="T4" t="n">
         <v>0.01565796903635935</v>
@@ -1058,7 +1058,7 @@
         <v>0.3009235992525693</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.3027558652251359</v>
+        <v>0.1437425571645632</v>
       </c>
       <c r="Z4" t="n">
         <v>2.216291768419251</v>
@@ -1183,10 +1183,10 @@
         <v>228.5347196553994</v>
       </c>
       <c r="R5" t="n">
-        <v>0.0664775994892856</v>
+        <v>0.04352984251314507</v>
       </c>
       <c r="S5" t="n">
-        <v>0.5284042060258277</v>
+        <v>0.3460015410949811</v>
       </c>
       <c r="T5" t="n">
         <v>0.03737690801709868</v>
@@ -1204,7 +1204,7 @@
         <v>0.2978263408351925</v>
       </c>
       <c r="Y5" t="n">
-        <v>0.3500564033205599</v>
+        <v>0.2292185672215481</v>
       </c>
       <c r="Z5" t="n">
         <v>2.679201724604715</v>
@@ -1329,10 +1329,10 @@
         <v>290.2632249120762</v>
       </c>
       <c r="R6" t="n">
-        <v>0.06984877902268166</v>
+        <v>0.03943152109889309</v>
       </c>
       <c r="S6" t="n">
-        <v>0.6131651556018852</v>
+        <v>0.3461482807361684</v>
       </c>
       <c r="T6" t="n">
         <v>0.03181025930014108</v>
@@ -1350,7 +1350,7 @@
         <v>0.3480613225914486</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.3677532865802214</v>
+        <v>0.2076066565782977</v>
       </c>
       <c r="Z6" t="n">
         <v>1.543004944765388</v>
@@ -1470,10 +1470,10 @@
         <v>279.9616300555159</v>
       </c>
       <c r="R7" t="n">
-        <v>0.06430391599122437</v>
+        <v>0.03441434570801764</v>
       </c>
       <c r="S7" t="n">
-        <v>0.5726907157049396</v>
+        <v>0.30649418422249</v>
       </c>
       <c r="T7" t="n">
         <v>0.02560648978976426</v>
@@ -1491,7 +1491,7 @@
         <v>0.3531250985305872</v>
       </c>
       <c r="Y7" t="n">
-        <v>0.3385686317849538</v>
+        <v>0.1811960867473147</v>
       </c>
       <c r="Z7" t="n">
         <v>1.953362366508123</v>
@@ -1616,10 +1616,10 @@
         <v>284.9053574958589</v>
       </c>
       <c r="R8" t="n">
-        <v>0.06499901301360293</v>
+        <v>0.03585933065495057</v>
       </c>
       <c r="S8" t="n">
-        <v>0.5894089955610178</v>
+        <v>0.3251712769607986</v>
       </c>
       <c r="T8" t="n">
         <v>0.02749958794557083</v>
@@ -1637,7 +1637,7 @@
         <v>0.3589072716637888</v>
       </c>
       <c r="Y8" t="n">
-        <v>0.3422240700784343</v>
+        <v>0.1888017297194542</v>
       </c>
       <c r="Z8" t="n">
         <v>1.973230055558392</v>
@@ -1757,10 +1757,10 @@
         <v>332.8525260660337</v>
       </c>
       <c r="R9" t="n">
-        <v>0.06851404236594695</v>
+        <v>0.03495730917238263</v>
       </c>
       <c r="S9" t="n">
-        <v>0.6662245329419215</v>
+        <v>0.339921805399886</v>
       </c>
       <c r="T9" t="n">
         <v>0.02566871865415921</v>
@@ -1778,7 +1778,7 @@
         <v>0.3996198518129659</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.3606834890571139</v>
+        <v>0.1840283218584391</v>
       </c>
       <c r="Z9" t="n">
         <v>1.712118408202441</v>
@@ -1903,10 +1903,10 @@
         <v>303.857374296533</v>
       </c>
       <c r="R10" t="n">
-        <v>0.06470426252881842</v>
+        <v>0.03020578966327735</v>
       </c>
       <c r="S10" t="n">
-        <v>0.5911847628142024</v>
+        <v>0.2759818580691952</v>
       </c>
       <c r="T10" t="n">
         <v>0.01904922973721497</v>
@@ -1924,7 +1924,7 @@
         <v>0.3807978093607899</v>
       </c>
       <c r="Y10" t="n">
-        <v>0.3406551225047579</v>
+        <v>0.159027497972236</v>
       </c>
       <c r="Z10" t="n">
         <v>1.750714081180046</v>
@@ -2044,10 +2044,10 @@
         <v>302.7588036307113</v>
       </c>
       <c r="R11" t="n">
-        <v>0.06433478094425596</v>
+        <v>0.03014587116587267</v>
       </c>
       <c r="S11" t="n">
-        <v>0.5895569933845924</v>
+        <v>0.2762535118120735</v>
       </c>
       <c r="T11" t="n">
         <v>0.0190082545813362</v>
@@ -2065,7 +2065,7 @@
         <v>0.3800020170877917</v>
       </c>
       <c r="Y11" t="n">
-        <v>0.3387108810435742</v>
+        <v>0.1587125102868709</v>
       </c>
       <c r="Z11" t="n">
         <v>1.773764720596302</v>
@@ -2185,10 +2185,10 @@
         <v>292.8154777280224</v>
       </c>
       <c r="R12" t="n">
-        <v>0.06450361844921461</v>
+        <v>0.03525570969913175</v>
       </c>
       <c r="S12" t="n">
-        <v>0.6006423729922843</v>
+        <v>0.3282927941769044</v>
       </c>
       <c r="T12" t="n">
         <v>0.02665320217099458</v>
@@ -2206,7 +2206,7 @@
         <v>0.3732018204301692</v>
       </c>
       <c r="Y12" t="n">
-        <v>0.3396087823592673</v>
+        <v>0.1856197982375317</v>
       </c>
       <c r="Z12" t="n">
         <v>2.185671274726886</v>
@@ -2326,10 +2326,10 @@
         <v>366.3081757600917</v>
       </c>
       <c r="R13" t="n">
-        <v>0.07030251835319687</v>
+        <v>0.03253848788546</v>
       </c>
       <c r="S13" t="n">
-        <v>0.7089814330309555</v>
+        <v>0.3281416414387209</v>
       </c>
       <c r="T13" t="n">
         <v>0.0216438467116082</v>
@@ -2347,7 +2347,7 @@
         <v>0.4326924435957378</v>
       </c>
       <c r="Y13" t="n">
-        <v>0.3700610809162503</v>
+        <v>0.1712773351557482</v>
       </c>
       <c r="Z13" t="n">
         <v>1.523822441374162</v>
@@ -2472,10 +2472,10 @@
         <v>380.5274144141753</v>
       </c>
       <c r="R14" t="n">
-        <v>0.0754346887517951</v>
+        <v>0.03726743461629045</v>
       </c>
       <c r="S14" t="n">
-        <v>0.7506422581779707</v>
+        <v>0.3708441267507243</v>
       </c>
       <c r="T14" t="n">
         <v>0.02786925035529117</v>
@@ -2493,7 +2493,7 @@
         <v>0.4466196204122587</v>
       </c>
       <c r="Y14" t="n">
-        <v>0.3970577879147413</v>
+        <v>0.1961607503769202</v>
       </c>
       <c r="Z14" t="n">
         <v>1.25015691391364</v>
@@ -2618,10 +2618,10 @@
         <v>323.8647870003163</v>
       </c>
       <c r="R15" t="n">
-        <v>0.07064820256765118</v>
+        <v>0.04288532275649014</v>
       </c>
       <c r="S15" t="n">
-        <v>0.6969518275469019</v>
+        <v>0.4230681458803355</v>
       </c>
       <c r="T15" t="n">
         <v>0.03587752092192817</v>
@@ -2639,7 +2639,7 @@
         <v>0.4071262227019383</v>
       </c>
       <c r="Y15" t="n">
-        <v>0.3719281292647166</v>
+        <v>0.2257701864454561</v>
       </c>
       <c r="Z15" t="n">
         <v>1.844836198763456</v>
@@ -2764,10 +2764,10 @@
         <v>365.3077092385499</v>
       </c>
       <c r="R16" t="n">
-        <v>0.07958725525516615</v>
+        <v>0.04574672100633774</v>
       </c>
       <c r="S16" t="n">
-        <v>0.7607455870596773</v>
+        <v>0.4372762450023384</v>
       </c>
       <c r="T16" t="n">
         <v>0.03846601920121103</v>
@@ -2785,7 +2785,7 @@
         <v>0.4573794417773399</v>
       </c>
       <c r="Y16" t="n">
-        <v>0.4189357595420255</v>
+        <v>0.2408040992229495</v>
       </c>
       <c r="Z16" t="n">
         <v>1.684038290222404</v>
@@ -2910,10 +2910,10 @@
         <v>434.9747725949474</v>
       </c>
       <c r="R17" t="n">
-        <v>0.07982341444126252</v>
+        <v>0.04101834882373358</v>
       </c>
       <c r="S17" t="n">
-        <v>0.8641796932101006</v>
+        <v>0.4440705067629318</v>
       </c>
       <c r="T17" t="n">
         <v>0.03216291235005606</v>
@@ -2931,7 +2931,7 @@
         <v>0.5036370135031565</v>
       </c>
       <c r="Y17" t="n">
-        <v>0.420077793118673</v>
+        <v>0.2158626960755375</v>
       </c>
       <c r="Z17" t="n">
         <v>1.226402369197755</v>
@@ -3056,10 +3056,10 @@
         <v>364.6266753510416</v>
       </c>
       <c r="R18" t="n">
-        <v>0.06953172073797809</v>
+        <v>0.02745753808882992</v>
       </c>
       <c r="S18" t="n">
-        <v>0.6753787264251591</v>
+        <v>0.2667018291563065</v>
       </c>
       <c r="T18" t="n">
         <v>0.01210608377023708</v>
@@ -3077,7 +3077,7 @@
         <v>0.4601753676917382</v>
       </c>
       <c r="Y18" t="n">
-        <v>0.366005672296658</v>
+        <v>0.1445328057633443</v>
       </c>
       <c r="Z18" t="n">
         <v>1.060831560138101</v>
@@ -3194,10 +3194,10 @@
         <v>454.9039090145141</v>
       </c>
       <c r="R19" t="n">
-        <v>0.07589220053415822</v>
+        <v>0.02991739940245386</v>
       </c>
       <c r="S19" t="n">
-        <v>0.8424606857495196</v>
+        <v>0.332105705712004</v>
       </c>
       <c r="T19" t="n">
         <v>0.01524845411825352</v>
@@ -3215,7 +3215,7 @@
         <v>0.5228162358938716</v>
       </c>
       <c r="Y19" t="n">
-        <v>0.3993587053442236</v>
+        <v>0.1574308533490535</v>
       </c>
       <c r="Z19" t="n">
         <v>1.177088983194154</v>
@@ -3340,10 +3340,10 @@
         <v>666.2793795323425</v>
       </c>
       <c r="R20" t="n">
-        <v>0.09559669160520061</v>
+        <v>0.0418583718204418</v>
       </c>
       <c r="S20" t="n">
-        <v>1.262512339164607</v>
+        <v>0.5528089940486279</v>
       </c>
       <c r="T20" t="n">
         <v>0.03042025127982355</v>
@@ -3361,7 +3361,7 @@
         <v>0.6586738663279574</v>
       </c>
       <c r="Y20" t="n">
-        <v>0.502492362472465</v>
+        <v>0.2200234316912323</v>
       </c>
       <c r="Z20" t="n">
         <v>0.6165669580640616</v>
@@ -3481,10 +3481,10 @@
         <v>710.0173888051944</v>
       </c>
       <c r="R21" t="n">
-        <v>0.0934159975242862</v>
+        <v>0.03176232743395979</v>
       </c>
       <c r="S21" t="n">
-        <v>1.28652987505091</v>
+        <v>0.4374323908955187</v>
       </c>
       <c r="T21" t="n">
         <v>0.0125010852298561</v>
@@ -3502,7 +3502,7 @@
         <v>0.6827936599692225</v>
       </c>
       <c r="Y21" t="n">
-        <v>0.4908770761478185</v>
+        <v>0.1669028735509503</v>
       </c>
       <c r="Z21" t="n">
         <v>0.4880538549496394</v>
@@ -3627,10 +3627,10 @@
         <v>896.5270268499016</v>
       </c>
       <c r="R22" t="n">
-        <v>0.1133385357079901</v>
+        <v>0.04028608025538834</v>
       </c>
       <c r="S22" t="n">
-        <v>1.636370933322566</v>
+        <v>0.5816465718002936</v>
       </c>
       <c r="T22" t="n">
         <v>0.02366121909755019</v>
@@ -3648,7 +3648,7 @@
         <v>0.7990404597704105</v>
       </c>
       <c r="Y22" t="n">
-        <v>0.5945026660785261</v>
+        <v>0.2113154362553971</v>
       </c>
       <c r="Z22" t="n">
         <v>0.3340915542427599</v>
@@ -3773,10 +3773,10 @@
         <v>544.3989324383406</v>
       </c>
       <c r="R23" t="n">
-        <v>0.08362419687089735</v>
+        <v>0.03456419819307398</v>
       </c>
       <c r="S23" t="n">
-        <v>1.015580980037545</v>
+        <v>0.4197677656543253</v>
       </c>
       <c r="T23" t="n">
         <v>0.02155741707058919</v>
@@ -3794,7 +3794,7 @@
         <v>0.5926520497047932</v>
       </c>
       <c r="Y23" t="n">
-        <v>0.4398711326682345</v>
+        <v>0.1818109300640468</v>
       </c>
       <c r="Z23" t="n">
         <v>0.9676569692153486</v>
@@ -3919,10 +3919,10 @@
         <v>544.0780004292803</v>
       </c>
       <c r="R24" t="n">
-        <v>0.08484679685627344</v>
+        <v>0.03394734640440935</v>
       </c>
       <c r="S24" t="n">
-        <v>1.007800920355075</v>
+        <v>0.4032228465610803</v>
       </c>
       <c r="T24" t="n">
         <v>0.02023942698494656</v>
@@ -3940,7 +3940,7 @@
         <v>0.5984242868416478</v>
       </c>
       <c r="Y24" t="n">
-        <v>0.4463028330505808</v>
+        <v>0.1785665156046148</v>
       </c>
       <c r="Z24" t="n">
         <v>0.906764956917385</v>
@@ -4062,10 +4062,10 @@
         <v>930.6619575046815</v>
       </c>
       <c r="R25" t="n">
-        <v>0.1122678179563154</v>
+        <v>0.04099880404070416</v>
       </c>
       <c r="S25" t="n">
-        <v>1.701951673694884</v>
+        <v>0.6215314809424405</v>
       </c>
       <c r="T25" t="n">
         <v>0.02473542485710895</v>
@@ -4083,7 +4083,7 @@
         <v>0.8292876502454331</v>
       </c>
       <c r="Y25" t="n">
-        <v>0.5886351013423641</v>
+        <v>0.2149621824912119</v>
       </c>
       <c r="Z25" t="n">
         <v>0.3687925877173285</v>
@@ -4208,10 +4208,10 @@
         <v>618.5008542055614</v>
       </c>
       <c r="R26" t="n">
-        <v>0.09242590072726238</v>
+        <v>0.04267242909523233</v>
       </c>
       <c r="S26" t="n">
-        <v>1.183025290588741</v>
+        <v>0.5461949781748147</v>
       </c>
       <c r="T26" t="n">
         <v>0.03203961011794775</v>
@@ -4229,7 +4229,7 @@
         <v>0.6495667435386698</v>
       </c>
       <c r="Y26" t="n">
-        <v>0.4859727216980054</v>
+        <v>0.2243704020810082</v>
       </c>
       <c r="Z26" t="n">
         <v>0.7940434459215121</v>
@@ -4354,10 +4354,10 @@
         <v>481.9153799252361</v>
       </c>
       <c r="R27" t="n">
-        <v>0.0771078006912097</v>
+        <v>0.03955111523473034</v>
       </c>
       <c r="S27" t="n">
-        <v>0.9516631475203478</v>
+        <v>0.48813918273919</v>
       </c>
       <c r="T27" t="n">
         <v>0.03017954165546297</v>
@@ -4375,7 +4375,7 @@
         <v>0.5511318973670239</v>
       </c>
       <c r="Y27" t="n">
-        <v>0.4057105330459299</v>
+        <v>0.2081022140509932</v>
       </c>
       <c r="Z27" t="n">
         <v>1.37647581175124</v>
@@ -4500,10 +4500,10 @@
         <v>606.7875476519142</v>
       </c>
       <c r="R28" t="n">
-        <v>0.09337061563043457</v>
+        <v>0.048173756260283</v>
       </c>
       <c r="S28" t="n">
-        <v>1.201509898115523</v>
+        <v>0.6199085717205879</v>
       </c>
       <c r="T28" t="n">
         <v>0.0392899701759272</v>
@@ -4521,7 +4521,7 @@
         <v>0.6414080638120929</v>
       </c>
       <c r="Y28" t="n">
-        <v>0.4909738348288294</v>
+        <v>0.2533136757160995</v>
       </c>
       <c r="Z28" t="n">
         <v>0.8528938169750084</v>
@@ -4646,10 +4646,10 @@
         <v>502.2349308672917</v>
       </c>
       <c r="R29" t="n">
-        <v>0.08260886882212626</v>
+        <v>0.04570153462045669</v>
       </c>
       <c r="S29" t="n">
-        <v>1.021799693961892</v>
+        <v>0.5652881434476649</v>
       </c>
       <c r="T29" t="n">
         <v>0.03759356235100123</v>
@@ -4667,7 +4667,7 @@
         <v>0.5684962285406479</v>
       </c>
       <c r="Y29" t="n">
-        <v>0.4346165797595717</v>
+        <v>0.2404420366689062</v>
       </c>
       <c r="Z29" t="n">
         <v>1.219684522050477</v>
@@ -4792,10 +4792,10 @@
         <v>1096.631622468331</v>
       </c>
       <c r="R30" t="n">
-        <v>0.1204621521253072</v>
+        <v>0.0417776904554347</v>
       </c>
       <c r="S30" t="n">
-        <v>1.993382389937878</v>
+        <v>0.6913284461289626</v>
       </c>
       <c r="T30" t="n">
         <v>0.02315724227631104</v>
@@ -4813,7 +4813,7 @@
         <v>0.9228914990693117</v>
       </c>
       <c r="Y30" t="n">
-        <v>0.6299082020291965</v>
+        <v>0.2184595693786099</v>
       </c>
       <c r="Z30" t="n">
         <v>0.2644084526834496</v>
@@ -4938,10 +4938,10 @@
         <v>550.3911770750043</v>
       </c>
       <c r="R31" t="n">
-        <v>0.08628712069705406</v>
+        <v>0.04680599631908023</v>
       </c>
       <c r="S31" t="n">
-        <v>1.110426231345523</v>
+        <v>0.6023448885198825</v>
       </c>
       <c r="T31" t="n">
         <v>0.03846411472934194</v>
@@ -4959,7 +4959,7 @@
         <v>0.6018582254089324</v>
       </c>
       <c r="Y31" t="n">
-        <v>0.4538647811562827</v>
+        <v>0.2461965714529446</v>
       </c>
       <c r="Z31" t="n">
         <v>1.270700200018976</v>
@@ -5084,10 +5084,10 @@
         <v>608.1527212277065</v>
       </c>
       <c r="R32" t="n">
-        <v>0.08759734310141581</v>
+        <v>0.04117625140448919</v>
       </c>
       <c r="S32" t="n">
-        <v>1.167711552991346</v>
+        <v>0.5488977493099449</v>
       </c>
       <c r="T32" t="n">
         <v>0.03058272662020578</v>
@@ -5105,7 +5105,7 @@
         <v>0.6427960171258907</v>
       </c>
       <c r="Y32" t="n">
-        <v>0.4606123913153962</v>
+        <v>0.2165167452952024</v>
       </c>
       <c r="Z32" t="n">
         <v>0.9403060490214101</v>
@@ -5230,10 +5230,10 @@
         <v>807.8285253071689</v>
       </c>
       <c r="R33" t="n">
-        <v>0.1064260239396567</v>
+        <v>0.04444684130520296</v>
       </c>
       <c r="S33" t="n">
-        <v>1.508680622038008</v>
+        <v>0.6300722859474562</v>
       </c>
       <c r="T33" t="n">
         <v>0.03170748900638904</v>
@@ -5251,7 +5251,7 @@
         <v>0.7748030583635716</v>
       </c>
       <c r="Y33" t="n">
-        <v>0.5587761230542826</v>
+        <v>0.2333624121917033</v>
       </c>
       <c r="Z33" t="n">
         <v>0.4698224901988813</v>
@@ -5376,10 +5376,10 @@
         <v>534.9018780626452</v>
       </c>
       <c r="R34" t="n">
-        <v>0.08311849227642856</v>
+        <v>0.04430684122059851</v>
       </c>
       <c r="S34" t="n">
-        <v>1.070715593749519</v>
+        <v>0.5707517605938608</v>
       </c>
       <c r="T34" t="n">
         <v>0.03561326596181213</v>
@@ -5397,7 +5397,7 @@
         <v>0.5935989896801104</v>
       </c>
       <c r="Y34" t="n">
-        <v>0.4372314146637333</v>
+        <v>0.2330689878461314</v>
       </c>
       <c r="Z34" t="n">
         <v>1.252485750795232</v>
@@ -5522,10 +5522,10 @@
         <v>1517.748845141926</v>
       </c>
       <c r="R35" t="n">
-        <v>0.1354523583268862</v>
+        <v>0.04551783099344783</v>
       </c>
       <c r="S35" t="n">
-        <v>2.784471221212604</v>
+        <v>0.9357023533499979</v>
       </c>
       <c r="T35" t="n">
         <v>0.02337377779883945</v>
@@ -5543,7 +5543,7 @@
         <v>1.118256327482045</v>
       </c>
       <c r="Y35" t="n">
-        <v>0.6980441304018469</v>
+        <v>0.2345729166037912</v>
       </c>
       <c r="Z35" t="n">
         <v>0.1252505675351251</v>
@@ -5660,10 +5660,10 @@
         <v>573.3997087785676</v>
       </c>
       <c r="R36" t="n">
-        <v>0.08441624072413377</v>
+        <v>0.03920528688627165</v>
       </c>
       <c r="S36" t="n">
-        <v>1.095359209252984</v>
+        <v>0.5087157598337078</v>
       </c>
       <c r="T36" t="n">
         <v>0.02827431025703319</v>
@@ -5681,7 +5681,7 @@
         <v>0.6293890251791517</v>
       </c>
       <c r="Y36" t="n">
-        <v>0.4439711594422189</v>
+        <v>0.2061927482893305</v>
       </c>
       <c r="Z36" t="n">
         <v>0.9941371187539264</v>
@@ -5806,10 +5806,10 @@
         <v>834.1299991188334</v>
       </c>
       <c r="R37" t="n">
-        <v>0.1020599536145249</v>
+        <v>0.04445981185618579</v>
       </c>
       <c r="S37" t="n">
-        <v>1.569503743256955</v>
+        <v>0.6837142156299462</v>
       </c>
       <c r="T37" t="n">
         <v>0.0321363995413614</v>
@@ -5827,7 +5827,7 @@
         <v>0.7948877954783655</v>
       </c>
       <c r="Y37" t="n">
-        <v>0.5357128806693283</v>
+        <v>0.2333696326519198</v>
       </c>
       <c r="Z37" t="n">
         <v>0.5692240977606092</v>
@@ -5952,10 +5952,10 @@
         <v>640.6799046401379</v>
       </c>
       <c r="R38" t="n">
-        <v>0.08959978692788791</v>
+        <v>0.04383290397509337</v>
       </c>
       <c r="S38" t="n">
-        <v>1.242135659418544</v>
+        <v>0.6076623053484728</v>
       </c>
       <c r="T38" t="n">
         <v>0.03375788602839082</v>
@@ -5973,7 +5973,7 @@
         <v>0.6762628747810386</v>
       </c>
       <c r="Y38" t="n">
-        <v>0.4710489581014726</v>
+        <v>0.2304407683987819</v>
       </c>
       <c r="Z38" t="n">
         <v>0.8976155480627297</v>
@@ -6098,10 +6098,10 @@
         <v>681.7347541629648</v>
       </c>
       <c r="R39" t="n">
-        <v>0.09522865523646261</v>
+        <v>0.04672635507840902</v>
       </c>
       <c r="S39" t="n">
-        <v>1.323261322660856</v>
+        <v>0.6492917312613846</v>
       </c>
       <c r="T39" t="n">
         <v>0.03679586790951254</v>
@@ -6119,7 +6119,7 @@
         <v>0.7061732995796922</v>
       </c>
       <c r="Y39" t="n">
-        <v>0.5005047411144811</v>
+        <v>0.2455853460670076</v>
       </c>
       <c r="Z39" t="n">
         <v>0.7637387563969605</v>
@@ -6244,10 +6244,10 @@
         <v>744.8250719255465</v>
       </c>
       <c r="R40" t="n">
-        <v>0.09643209795178394</v>
+        <v>0.04629650430838572</v>
       </c>
       <c r="S40" t="n">
-        <v>1.435841770397525</v>
+        <v>0.6893395054269839</v>
       </c>
       <c r="T40" t="n">
         <v>0.03580323589234279</v>
@@ -6265,7 +6265,7 @@
         <v>0.7447515781791074</v>
       </c>
       <c r="Y40" t="n">
-        <v>0.5065875211408369</v>
+        <v>0.2432098010228692</v>
       </c>
       <c r="Z40" t="n">
         <v>0.7387211964130875</v>
@@ -6390,10 +6390,10 @@
         <v>679.1989776779841</v>
       </c>
       <c r="R41" t="n">
-        <v>0.0892844761675672</v>
+        <v>0.03418103522859745</v>
       </c>
       <c r="S41" t="n">
-        <v>1.242618805692191</v>
+        <v>0.4757153650469784</v>
       </c>
       <c r="T41" t="n">
         <v>0.0184704960795956</v>
@@ -6411,7 +6411,7 @@
         <v>0.7085045505948163</v>
       </c>
       <c r="Y41" t="n">
-        <v>0.4692714997195238</v>
+        <v>0.1796525706617343</v>
       </c>
       <c r="Z41" t="n">
         <v>0.7701663629538618</v>
@@ -6531,10 +6531,10 @@
         <v>1368.859627295949</v>
       </c>
       <c r="R42" t="n">
-        <v>0.1275416037607389</v>
+        <v>0.03896831800451564</v>
       </c>
       <c r="S42" t="n">
-        <v>2.460293924730256</v>
+        <v>0.7517038614577872</v>
       </c>
       <c r="T42" t="n">
         <v>0.009916333757339949</v>
@@ -6552,7 +6552,7 @@
         <v>1.081453942752446</v>
       </c>
       <c r="Y42" t="n">
-        <v>0.6618415736852944</v>
+        <v>0.2022152156747209</v>
       </c>
       <c r="Z42" t="n">
         <v>0.8790383170548457</v>
@@ -6669,10 +6669,10 @@
         <v>948.0447993486778</v>
       </c>
       <c r="R43" t="n">
-        <v>0.1078179411597709</v>
+        <v>0.03842172599078816</v>
       </c>
       <c r="S43" t="n">
-        <v>1.718620296329172</v>
+        <v>0.6124431369906795</v>
       </c>
       <c r="T43" t="n">
         <v>0.02029819873586015</v>
@@ -6690,7 +6690,7 @@
         <v>0.8731019981734591</v>
       </c>
       <c r="Y43" t="n">
-        <v>0.5651728420456273</v>
+        <v>0.2014035497332829</v>
       </c>
       <c r="Z43" t="n">
         <v>0.4194914960754469</v>
@@ -6807,10 +6807,10 @@
         <v>731.1582382711508</v>
       </c>
       <c r="R44" t="n">
-        <v>0.09284897445154126</v>
+        <v>0.0350806404281435</v>
       </c>
       <c r="S44" t="n">
-        <v>1.334292731385979</v>
+        <v>0.5041288157691655</v>
       </c>
       <c r="T44" t="n">
         <v>0.01894581618138158</v>
@@ -6828,7 +6828,7 @@
         <v>0.7457998722046391</v>
       </c>
       <c r="Y44" t="n">
-        <v>0.4878179725219298</v>
+        <v>0.1843097028213189</v>
       </c>
       <c r="Z44" t="n">
         <v>0.681491323520846</v>
@@ -6948,10 +6948,10 @@
         <v>1237.620054224844</v>
       </c>
       <c r="R45" t="n">
-        <v>0.1219206814901367</v>
+        <v>0.04106263354456815</v>
       </c>
       <c r="S45" t="n">
-        <v>2.238593032004605</v>
+        <v>0.7539535065350276</v>
       </c>
       <c r="T45" t="n">
         <v>0.01957389632763329</v>
@@ -6969,7 +6969,7 @@
         <v>1.023595129324798</v>
       </c>
       <c r="Y45" t="n">
-        <v>0.6354176923219358</v>
+        <v>0.2140073655154365</v>
       </c>
       <c r="Z45" t="n">
         <v>0.2642243398515706</v>
@@ -7094,10 +7094,10 @@
         <v>866.3086696679782</v>
       </c>
       <c r="R46" t="n">
-        <v>0.0986700882923523</v>
+        <v>0.04122943311199977</v>
       </c>
       <c r="S46" t="n">
-        <v>1.61101380428258</v>
+        <v>0.6731643503690377</v>
       </c>
       <c r="T46" t="n">
         <v>0.02743635952506665</v>
@@ -7115,7 +7115,7 @@
         <v>0.828132466475922</v>
       </c>
       <c r="Y46" t="n">
-        <v>0.51774166537541</v>
+        <v>0.2163390722692333</v>
       </c>
       <c r="Z46" t="n">
         <v>0.6267989512448702</v>
@@ -7240,10 +7240,10 @@
         <v>1285.62119037289</v>
       </c>
       <c r="R47" t="n">
-        <v>0.1164759574687055</v>
+        <v>0.03888274087244756</v>
       </c>
       <c r="S47" t="n">
-        <v>2.322456138185965</v>
+        <v>0.7752969983781646</v>
       </c>
       <c r="T47" t="n">
         <v>0.01529536919543423</v>
@@ -7261,7 +7261,7 @@
         <v>1.049191794337178</v>
       </c>
       <c r="Y47" t="n">
-        <v>0.6061775248950435</v>
+        <v>0.2023580156405093</v>
       </c>
       <c r="Z47" t="n">
         <v>0.2657888411605542</v>
@@ -7386,10 +7386,10 @@
         <v>816.8790944553372</v>
       </c>
       <c r="R48" t="n">
-        <v>0.1029112099160411</v>
+        <v>0.05044174127473233</v>
       </c>
       <c r="S48" t="n">
-        <v>1.581869475644106</v>
+        <v>0.7753504296172796</v>
       </c>
       <c r="T48" t="n">
         <v>0.04011589927875898</v>
@@ -7407,7 +7407,7 @@
         <v>0.8082051319580108</v>
       </c>
       <c r="Y48" t="n">
-        <v>0.5402745923782476</v>
+        <v>0.264814603076658</v>
       </c>
       <c r="Z48" t="n">
         <v>0.5953509816737408</v>
@@ -7532,10 +7532,10 @@
         <v>720.7862659486707</v>
       </c>
       <c r="R49" t="n">
-        <v>0.09638532769903818</v>
+        <v>0.05566754919762874</v>
       </c>
       <c r="S49" t="n">
-        <v>1.48893930473073</v>
+        <v>0.8599400342051043</v>
       </c>
       <c r="T49" t="n">
         <v>0.04774883620073907</v>
@@ -7553,7 +7553,7 @@
         <v>0.7407261599323092</v>
       </c>
       <c r="Y49" t="n">
-        <v>0.5064386272948836</v>
+        <v>0.2924946967918938</v>
       </c>
       <c r="Z49" t="n">
         <v>0.8906056203022326</v>
@@ -7678,10 +7678,10 @@
         <v>1477.380913247307</v>
       </c>
       <c r="R50" t="n">
-        <v>0.1565967371373412</v>
+        <v>0.1042444451707642</v>
       </c>
       <c r="S50" t="n">
-        <v>3.392046536356433</v>
+        <v>2.258041997808464</v>
       </c>
       <c r="T50" t="n">
         <v>0.09707869293436806</v>
@@ -7699,7 +7699,7 @@
         <v>1.153308871514485</v>
       </c>
       <c r="Y50" t="n">
-        <v>0.8087308063199096</v>
+        <v>0.5383617547751618</v>
       </c>
       <c r="Z50" t="n">
         <v>0.2042709017828808</v>
@@ -7824,10 +7824,10 @@
         <v>796.81431764461</v>
       </c>
       <c r="R51" t="n">
-        <v>0.1499426500333533</v>
+        <v>0.1244224009475203</v>
       </c>
       <c r="S51" t="n">
-        <v>2.405408648434265</v>
+        <v>1.996007935244224</v>
       </c>
       <c r="T51" t="n">
         <v>0.1208057553173233</v>
@@ -7845,7 +7845,7 @@
         <v>0.8006128553838092</v>
       </c>
       <c r="Y51" t="n">
-        <v>0.787336622293173</v>
+        <v>0.653331876406324</v>
       </c>
       <c r="Z51" t="n">
         <v>0.7444129683581038</v>
@@ -7970,10 +7970,10 @@
         <v>1210.708556526963</v>
       </c>
       <c r="R52" t="n">
-        <v>0.1565763778164347</v>
+        <v>0.1150111600444982</v>
       </c>
       <c r="S52" t="n">
-        <v>3.026054616710419</v>
+        <v>2.222749412646996</v>
       </c>
       <c r="T52" t="n">
         <v>0.1095387665008975</v>
@@ -7991,7 +7991,7 @@
         <v>1.03109617197945</v>
       </c>
       <c r="Y52" t="n">
-        <v>0.8166277893947194</v>
+        <v>0.5998434163100338</v>
       </c>
       <c r="Z52" t="n">
         <v>0.3006126699157793</v>
@@ -8116,10 +8116,10 @@
         <v>1230.299326711783</v>
       </c>
       <c r="R53" t="n">
-        <v>0.1460321000327657</v>
+        <v>0.09973917527164307</v>
       </c>
       <c r="S53" t="n">
-        <v>2.856647815559146</v>
+        <v>1.951075805261182</v>
       </c>
       <c r="T53" t="n">
         <v>0.09329295925735386</v>
@@ -8137,7 +8137,7 @@
         <v>1.04549216297946</v>
       </c>
       <c r="Y53" t="n">
-        <v>0.7612342127995915</v>
+        <v>0.5199190627002842</v>
       </c>
       <c r="Z53" t="n">
         <v>0.3122784966545478</v>
@@ -8262,10 +8262,10 @@
         <v>1101.247854762019</v>
       </c>
       <c r="R54" t="n">
-        <v>0.1240834860372098</v>
+        <v>0.07125152259779147</v>
       </c>
       <c r="S54" t="n">
-        <v>2.274203749153245</v>
+        <v>1.305898834726341</v>
       </c>
       <c r="T54" t="n">
         <v>0.06267727567761784</v>
@@ -8283,7 +8283,7 @@
         <v>0.981750301436303</v>
       </c>
       <c r="Y54" t="n">
-        <v>0.6487851211933646</v>
+        <v>0.372546977846492</v>
       </c>
       <c r="Z54" t="n">
         <v>0.3682336438301901</v>
@@ -8408,10 +8408,10 @@
         <v>958.1495376201941</v>
       </c>
       <c r="R55" t="n">
-        <v>0.1267231839568623</v>
+        <v>0.085859782096355</v>
       </c>
       <c r="S55" t="n">
-        <v>2.196804382813472</v>
+        <v>1.488418612342389</v>
       </c>
       <c r="T55" t="n">
         <v>0.07968005938665459</v>
@@ -8429,7 +8429,7 @@
         <v>0.9032573190295105</v>
       </c>
       <c r="Y55" t="n">
-        <v>0.6641800031877484</v>
+        <v>0.4500072407103402</v>
       </c>
       <c r="Z55" t="n">
         <v>0.5543013734981523</v>
@@ -8554,10 +8554,10 @@
         <v>1140.32678451486</v>
       </c>
       <c r="R56" t="n">
-        <v>0.1437553033308938</v>
+        <v>0.1008042152759123</v>
       </c>
       <c r="S56" t="n">
-        <v>2.705175899339792</v>
+        <v>1.896925730027346</v>
       </c>
       <c r="T56" t="n">
         <v>0.09480260607209692</v>
@@ -8575,7 +8575,7 @@
         <v>1.004787008460192</v>
       </c>
       <c r="Y56" t="n">
-        <v>0.7510267160172936</v>
+        <v>0.5266355884284026</v>
       </c>
       <c r="Z56" t="n">
         <v>0.3861022322764417</v>
@@ -8700,10 +8700,10 @@
         <v>991.4228377102024</v>
       </c>
       <c r="R57" t="n">
-        <v>0.2074327560042446</v>
+        <v>0.1841414008573738</v>
       </c>
       <c r="S57" t="n">
-        <v>3.631403270487753</v>
+        <v>3.22365521331636</v>
       </c>
       <c r="T57" t="n">
         <v>0.1812469917955691</v>
@@ -8721,7 +8721,7 @@
         <v>0.9270861107020413</v>
       </c>
       <c r="Y57" t="n">
-        <v>1.086667330329878</v>
+        <v>0.9646521037824507</v>
       </c>
       <c r="Z57" t="n">
         <v>0.4979930645837926</v>
@@ -8846,10 +8846,10 @@
         <v>1087.292633970525</v>
       </c>
       <c r="R58" t="n">
-        <v>0.2031876065845885</v>
+        <v>0.1768661525658967</v>
       </c>
       <c r="S58" t="n">
-        <v>3.726593124002803</v>
+        <v>3.243840503365099</v>
       </c>
       <c r="T58" t="n">
         <v>0.1736120024272776</v>
@@ -8867,7 +8867,7 @@
         <v>0.9897207938221579</v>
       </c>
       <c r="Y58" t="n">
-        <v>1.06268095705719</v>
+        <v>0.9250184863096168</v>
       </c>
       <c r="Z58" t="n">
         <v>0.4074737942111886</v>
@@ -8992,10 +8992,10 @@
         <v>1100.714171040751</v>
       </c>
       <c r="R59" t="n">
-        <v>0.2493385128292472</v>
+        <v>0.2285593781446843</v>
       </c>
       <c r="S59" t="n">
-        <v>4.646615009386353</v>
+        <v>4.259379848593236</v>
       </c>
       <c r="T59" t="n">
         <v>0.2260446327550389</v>
@@ -9013,7 +9013,7 @@
         <v>0.9971193390270346</v>
       </c>
       <c r="Y59" t="n">
-        <v>1.303709646453764</v>
+        <v>1.195062337917925</v>
       </c>
       <c r="Z59" t="n">
         <v>0.4424502235139683</v>
@@ -9138,10 +9138,10 @@
         <v>1055.998480826153</v>
       </c>
       <c r="R60" t="n">
-        <v>0.2461313503076235</v>
+        <v>0.2259369826376492</v>
       </c>
       <c r="S60" t="n">
-        <v>4.486880318165957</v>
+        <v>4.118744724211886</v>
       </c>
       <c r="T60" t="n">
         <v>0.2234692596964148</v>
@@ -9159,7 +9159,7 @@
         <v>0.9743027756802667</v>
       </c>
       <c r="Y60" t="n">
-        <v>1.288025591533263</v>
+        <v>1.182346805262235</v>
       </c>
       <c r="Z60" t="n">
         <v>0.4698220463213008</v>
@@ -9284,10 +9284,10 @@
         <v>1119.488754117979</v>
       </c>
       <c r="R61" t="n">
-        <v>0.3781710184204351</v>
+        <v>0.3647210152356247</v>
       </c>
       <c r="S61" t="n">
-        <v>7.132816719220564</v>
+        <v>6.879131473876016</v>
       </c>
       <c r="T61" t="n">
         <v>0.3631171171852328</v>
@@ -9305,7 +9305,7 @@
         <v>1.025535752483008</v>
       </c>
       <c r="Y61" t="n">
-        <v>1.97657608272104</v>
+        <v>1.9062773202229</v>
       </c>
       <c r="Z61" t="n">
         <v>0.4255055133414155</v>
@@ -9430,10 +9430,10 @@
         <v>1048.540959466458</v>
       </c>
       <c r="R62" t="n">
-        <v>1.458486534612809</v>
+        <v>1.455246719962166</v>
       </c>
       <c r="S62" t="n">
-        <v>26.47051264071681</v>
+        <v>26.41171226606257</v>
       </c>
       <c r="T62" t="n">
         <v>1.45486360552399</v>
@@ -9451,7 +9451,7 @@
         <v>0.9882110579130742</v>
       </c>
       <c r="Y62" t="n">
-        <v>7.633385028099329</v>
+        <v>7.616428579026184</v>
       </c>
       <c r="Z62" t="n">
         <v>2.834777491750536</v>
@@ -9552,10 +9552,10 @@
         <v>1017.504217633747</v>
       </c>
       <c r="R63" t="n">
-        <v>0.3748063200948277</v>
+        <v>0.3627983940667324</v>
       </c>
       <c r="S63" t="n">
-        <v>6.807184441663727</v>
+        <v>6.589098025152878</v>
       </c>
       <c r="T63" t="n">
         <v>0.361308821888685</v>
@@ -9573,7 +9573,7 @@
         <v>0.9724688889891336</v>
       </c>
       <c r="Y63" t="n">
-        <v>1.962675853830904</v>
+        <v>1.899796267211427</v>
       </c>
       <c r="Z63" t="n">
         <v>0.5265930441298312</v>
@@ -9687,10 +9687,10 @@
         <v>1130.45330750387</v>
       </c>
       <c r="R64" t="n">
-        <v>0.404819978484279</v>
+        <v>0.3925781010268457</v>
       </c>
       <c r="S64" t="n">
-        <v>7.796126269541819</v>
+        <v>7.560369074969187</v>
       </c>
       <c r="T64" t="n">
         <v>0.3910911829673833</v>
@@ -9708,7 +9708,7 @@
         <v>1.034969981867021</v>
       </c>
       <c r="Y64" t="n">
-        <v>2.115370844825805</v>
+        <v>2.051401396587741</v>
       </c>
       <c r="Z64" t="n">
         <v>0.4737852531373214</v>
@@ -9833,10 +9833,10 @@
         <v>1079.234183124676</v>
       </c>
       <c r="R65" t="n">
-        <v>0.3915143565030267</v>
+        <v>0.3800657009761729</v>
       </c>
       <c r="S65" t="n">
-        <v>7.556336498423256</v>
+        <v>7.335374247158348</v>
       </c>
       <c r="T65" t="n">
         <v>0.3786125670197011</v>
@@ -9854,7 +9854,7 @@
         <v>1.004709704806168</v>
       </c>
       <c r="Y65" t="n">
-        <v>2.047953626483768</v>
+        <v>1.988067404650157</v>
       </c>
       <c r="Z65" t="n">
         <v>0.5694848542965316</v>
@@ -9979,10 +9979,10 @@
         <v>1429.849882102506</v>
       </c>
       <c r="R66" t="n">
-        <v>0.3676357253206194</v>
+        <v>0.3502335221737565</v>
       </c>
       <c r="S66" t="n">
-        <v>7.985730464721332</v>
+        <v>7.607722305416423</v>
       </c>
       <c r="T66" t="n">
         <v>0.3481896288141496</v>
@@ -10000,7 +10000,7 @@
         <v>1.195810221256678</v>
       </c>
       <c r="Y66" t="n">
-        <v>1.902910142862398</v>
+        <v>1.812835031561837</v>
       </c>
       <c r="Z66" t="n">
         <v>0.3068154242362686</v>
@@ -10119,10 +10119,10 @@
         <v>1550.805148256374</v>
       </c>
       <c r="R67" t="n">
-        <v>0.3055173026102699</v>
+        <v>0.2822845769326371</v>
       </c>
       <c r="S67" t="n">
-        <v>6.926857774771263</v>
+        <v>6.400112529528877</v>
       </c>
       <c r="T67" t="n">
         <v>0.2795387241448997</v>
@@ -10140,7 +10140,7 @@
         <v>1.255401362211165</v>
       </c>
       <c r="Y67" t="n">
-        <v>1.571464885779468</v>
+        <v>1.45196457502319</v>
       </c>
       <c r="Z67" t="n">
         <v>0.2548256445536423</v>
@@ -10265,10 +10265,10 @@
         <v>1246.375922199096</v>
       </c>
       <c r="R68" t="n">
-        <v>0.4217920546580924</v>
+        <v>0.4096538921333197</v>
       </c>
       <c r="S68" t="n">
-        <v>8.794883604371812</v>
+        <v>8.541787972537639</v>
       </c>
       <c r="T68" t="n">
         <v>0.4081188252570417</v>
@@ -10286,7 +10286,7 @@
         <v>1.125364378941089</v>
       </c>
       <c r="Y68" t="n">
-        <v>2.197722731081284</v>
+        <v>2.134477548058868</v>
       </c>
       <c r="Z68" t="n">
         <v>0.4803640769736678</v>

</xml_diff>